<commit_message>
Ran some models and got some outputs
</commit_message>
<xml_diff>
--- a/Raw Data/Fish and Seal Plate Collated Raw (Plate 2).xlsx
+++ b/Raw Data/Fish and Seal Plate Collated Raw (Plate 2).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60d52dd049abb4b4/Pictures/Documents/MSc_Seal_SIA/Raw Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{9000E122-6165-4E04-8EEC-F80BBD745AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F526A3E8-352D-4890-AFFD-8CDC319D23F7}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{9000E122-6165-4E04-8EEC-F80BBD745AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33D2AE43-D6E5-4069-8269-178338A16334}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{60217609-3FF6-4791-BC76-FEC9C203F6A0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>FS1LE</t>
   </si>
@@ -126,15 +126,6 @@
   </si>
   <si>
     <t>C/N</t>
-  </si>
-  <si>
-    <t>‰air</t>
-  </si>
-  <si>
-    <t>‰ V-PDB</t>
-  </si>
-  <si>
-    <t>ratio</t>
   </si>
   <si>
     <r>
@@ -677,7 +668,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -801,15 +792,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -855,7 +837,7 @@
     <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -870,12 +852,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1237,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24BA6998-D5F9-4D82-B300-F953605826D9}">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:F82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1250,10 +1226,10 @@
         <v>26</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>27</v>
@@ -1265,1397 +1241,1383 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
-        <v>32</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2">
+        <v>14.120327104212071</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-17.862154989586763</v>
+      </c>
+      <c r="D2" s="2">
+        <v>14.510171235955157</v>
+      </c>
+      <c r="E2" s="2">
+        <v>48.432740001869391</v>
+      </c>
+      <c r="F2" s="3">
+        <v>3.3378475838973256</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2">
-        <v>14.120327104212071</v>
+        <v>15.076102108302791</v>
       </c>
       <c r="C3" s="2">
-        <v>-17.862154989586763</v>
+        <v>-17.098746108167973</v>
       </c>
       <c r="D3" s="2">
-        <v>14.510171235955157</v>
+        <v>14.498389984308421</v>
       </c>
       <c r="E3" s="2">
-        <v>48.432740001869391</v>
+        <v>47.73182722834251</v>
       </c>
       <c r="F3" s="3">
-        <v>3.3378475838973256</v>
+        <v>3.2922157067096811</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2">
-        <v>15.076102108302791</v>
+        <v>14.030380276324195</v>
       </c>
       <c r="C4" s="2">
-        <v>-17.098746108167973</v>
+        <v>-17.539870775029943</v>
       </c>
       <c r="D4" s="2">
-        <v>14.498389984308421</v>
+        <v>14.565190684145101</v>
       </c>
       <c r="E4" s="2">
-        <v>47.73182722834251</v>
+        <v>47.369725237766424</v>
       </c>
       <c r="F4" s="3">
-        <v>3.2922157067096811</v>
+        <v>3.252255755863918</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2">
-        <v>14.030380276324195</v>
+        <v>14.230046091979309</v>
       </c>
       <c r="C5" s="2">
-        <v>-17.539870775029943</v>
+        <v>-17.272795357696992</v>
       </c>
       <c r="D5" s="2">
-        <v>14.565190684145101</v>
+        <v>14.639828951011179</v>
       </c>
       <c r="E5" s="2">
-        <v>47.369725237766424</v>
+        <v>48.166322141663606</v>
       </c>
       <c r="F5" s="3">
-        <v>3.252255755863918</v>
+        <v>3.2900877669295951</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2">
-        <v>14.230046091979309</v>
+        <v>8.1235631708853617</v>
       </c>
       <c r="C6" s="2">
-        <v>-17.272795357696992</v>
+        <v>-19.119099288344209</v>
       </c>
       <c r="D6" s="2">
-        <v>14.639828951011179</v>
+        <v>9.1405192958276658</v>
       </c>
       <c r="E6" s="2">
-        <v>48.166322141663606</v>
+        <v>41.679852982267953</v>
       </c>
       <c r="F6" s="3">
-        <v>3.2900877669295951</v>
+        <v>4.5598998955445973</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2">
-        <v>8.1235631708853617</v>
+        <v>9.8697949530412998</v>
       </c>
       <c r="C7" s="2">
-        <v>-19.119099288344209</v>
+        <v>-16.735108739428185</v>
       </c>
       <c r="D7" s="2">
-        <v>9.1405192958276658</v>
+        <v>12.85427357072941</v>
       </c>
       <c r="E7" s="2">
-        <v>41.679852982267953</v>
+        <v>42.475296530113063</v>
       </c>
       <c r="F7" s="3">
-        <v>4.5598998955445973</v>
+        <v>3.3043716003395143</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2">
-        <v>9.8697949530412998</v>
+        <v>10.468670198890528</v>
       </c>
       <c r="C8" s="2">
-        <v>-16.735108739428185</v>
+        <v>-17.917730691340395</v>
       </c>
       <c r="D8" s="2">
-        <v>12.85427357072941</v>
+        <v>10.954449668190934</v>
       </c>
       <c r="E8" s="2">
-        <v>42.475296530113063</v>
+        <v>37.624359351473942</v>
       </c>
       <c r="F8" s="3">
-        <v>3.3043716003395143</v>
+        <v>3.4346188527138848</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2">
-        <v>10.468670198890528</v>
+        <v>10.376183907987446</v>
       </c>
       <c r="C9" s="2">
-        <v>-17.917730691340395</v>
+        <v>-17.220729387936618</v>
       </c>
       <c r="D9" s="2">
-        <v>10.954449668190934</v>
+        <v>12.773210715325536</v>
       </c>
       <c r="E9" s="2">
-        <v>37.624359351473942</v>
+        <v>42.876541237311656</v>
       </c>
       <c r="F9" s="3">
-        <v>3.4346188527138848</v>
+        <v>3.3567551802670557</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2">
-        <v>10.376183907987446</v>
+        <v>10.650775955253655</v>
       </c>
       <c r="C10" s="2">
-        <v>-17.220729387936618</v>
+        <v>-17.760536305253758</v>
       </c>
       <c r="D10" s="2">
-        <v>12.773210715325536</v>
+        <v>12.62046689726794</v>
       </c>
       <c r="E10" s="2">
-        <v>42.876541237311656</v>
+        <v>41.652959253793618</v>
       </c>
       <c r="F10" s="3">
-        <v>3.3567551802670557</v>
+        <v>3.300429341707682</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2">
-        <v>10.650775955253655</v>
+        <v>11.176299887238228</v>
       </c>
       <c r="C11" s="2">
-        <v>-17.760536305253758</v>
+        <v>-17.360355103881453</v>
       </c>
       <c r="D11" s="2">
-        <v>12.62046689726794</v>
+        <v>12.930282143342682</v>
       </c>
       <c r="E11" s="2">
-        <v>41.652959253793618</v>
+        <v>41.443204037253921</v>
       </c>
       <c r="F11" s="3">
-        <v>3.300429341707682</v>
+        <v>3.2051275894696136</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="2">
-        <v>11.176299887238228</v>
-      </c>
-      <c r="C12" s="2">
-        <v>-17.360355103881453</v>
-      </c>
-      <c r="D12" s="2">
-        <v>12.930282143342682</v>
-      </c>
-      <c r="E12" s="2">
-        <v>41.443204037253921</v>
-      </c>
-      <c r="F12" s="3">
-        <v>3.2051275894696136</v>
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>9.9365868992415951</v>
+      </c>
+      <c r="C12">
+        <v>-17.114996483607257</v>
+      </c>
+      <c r="D12">
+        <v>12.919809409342724</v>
+      </c>
+      <c r="E12">
+        <v>42.432714438939385</v>
+      </c>
+      <c r="F12">
+        <v>3.2843142723339978</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B13">
-        <v>9.9365868992415951</v>
+        <v>10.033581084030629</v>
       </c>
       <c r="C13">
-        <v>-17.114996483607257</v>
+        <v>-18.343483401822347</v>
       </c>
       <c r="D13">
-        <v>12.919809409342724</v>
+        <v>11.672657736149409</v>
       </c>
       <c r="E13">
-        <v>42.432714438939385</v>
+        <v>39.231496366956556</v>
       </c>
       <c r="F13">
-        <v>3.2843142723339978</v>
+        <v>3.3609737605394989</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>10.033581084030629</v>
+        <v>11.050284376163066</v>
       </c>
       <c r="C14">
-        <v>-18.343483401822347</v>
+        <v>-17.442054457390334</v>
       </c>
       <c r="D14">
-        <v>11.672657736149409</v>
+        <v>12.731423981452261</v>
       </c>
       <c r="E14">
-        <v>39.231496366956556</v>
+        <v>42.323018320370956</v>
       </c>
       <c r="F14">
-        <v>3.3609737605394989</v>
+        <v>3.3242957254450975</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15">
-        <v>11.050284376163066</v>
+        <v>10.595312348031349</v>
       </c>
       <c r="C15">
-        <v>-17.442054457390334</v>
+        <v>-17.770633219921006</v>
       </c>
       <c r="D15">
-        <v>12.731423981452261</v>
+        <v>12.926849044850032</v>
       </c>
       <c r="E15">
-        <v>42.323018320370956</v>
+        <v>43.172445228897381</v>
       </c>
       <c r="F15">
-        <v>3.3242957254450975</v>
+        <v>3.3397500875201285</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16">
-        <v>10.595312348031349</v>
+        <v>10.629046275455689</v>
       </c>
       <c r="C16">
-        <v>-17.770633219921006</v>
+        <v>-18.30113344944051</v>
       </c>
       <c r="D16">
-        <v>12.926849044850032</v>
+        <v>12.441275076902643</v>
       </c>
       <c r="E16">
-        <v>43.172445228897381</v>
+        <v>44.33037728905331</v>
       </c>
       <c r="F16">
-        <v>3.3397500875201285</v>
+        <v>3.5631699335507112</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B17">
-        <v>10.629046275455689</v>
+        <v>10.804837332249129</v>
       </c>
       <c r="C17">
-        <v>-18.30113344944051</v>
+        <v>-18.081337559448851</v>
       </c>
       <c r="D17">
-        <v>12.441275076902643</v>
+        <v>11.499279064530745</v>
       </c>
       <c r="E17">
-        <v>44.33037728905331</v>
+        <v>38.10867080896633</v>
       </c>
       <c r="F17">
-        <v>3.5631699335507112</v>
+        <v>3.3140052167715131</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18">
-        <v>10.804837332249129</v>
+        <v>9.1702131184678848</v>
       </c>
       <c r="C18">
-        <v>-18.081337559448851</v>
+        <v>-18.012164702917222</v>
       </c>
       <c r="D18">
-        <v>11.499279064530745</v>
+        <v>11.411909574515454</v>
       </c>
       <c r="E18">
-        <v>38.10867080896633</v>
+        <v>43.982550382803332</v>
       </c>
       <c r="F18">
-        <v>3.3140052167715131</v>
+        <v>3.8540920864833281</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B19">
-        <v>9.1702131184678848</v>
+        <v>10.47609750717049</v>
       </c>
       <c r="C19">
-        <v>-18.012164702917222</v>
+        <v>-17.759488586891912</v>
       </c>
       <c r="D19">
-        <v>11.411909574515454</v>
+        <v>12.190535051522417</v>
       </c>
       <c r="E19">
-        <v>43.982550382803332</v>
+        <v>44.891614508094754</v>
       </c>
       <c r="F19">
-        <v>3.8540920864833281</v>
+        <v>3.6824974718799122</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B20">
-        <v>10.47609750717049</v>
+        <v>10.750633981475577</v>
       </c>
       <c r="C20">
-        <v>-17.759488586891912</v>
+        <v>-17.700417318140538</v>
       </c>
       <c r="D20">
-        <v>12.190535051522417</v>
+        <v>12.162425989021656</v>
       </c>
       <c r="E20">
-        <v>44.891614508094754</v>
+        <v>38.816677754177604</v>
       </c>
       <c r="F20">
-        <v>3.6824974718799122</v>
+        <v>3.1915242723133734</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B21">
-        <v>10.750633981475577</v>
+        <v>14.510046569879531</v>
       </c>
       <c r="C21">
-        <v>-17.700417318140538</v>
+        <v>-18.264866914798226</v>
       </c>
       <c r="D21">
-        <v>12.162425989021656</v>
+        <v>11.467984413085578</v>
       </c>
       <c r="E21">
-        <v>38.816677754177604</v>
+        <v>43.414460534215721</v>
       </c>
       <c r="F21">
-        <v>3.1915242723133734</v>
+        <v>3.7857097612268746</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B22">
-        <v>14.510046569879531</v>
+        <v>13.818905607083654</v>
       </c>
       <c r="C22">
-        <v>-18.264866914798226</v>
+        <v>-18.586553226812796</v>
       </c>
       <c r="D22">
-        <v>11.467984413085578</v>
+        <v>11.537419984415683</v>
       </c>
       <c r="E22">
-        <v>43.414460534215721</v>
+        <v>43.357949278175646</v>
       </c>
       <c r="F22">
-        <v>3.7857097612268746</v>
+        <v>3.7580281671935274</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B23">
-        <v>13.818905607083654</v>
+        <v>13.738862557574727</v>
       </c>
       <c r="C23">
-        <v>-18.586553226812796</v>
+        <v>-18.704924205136475</v>
       </c>
       <c r="D23">
-        <v>11.537419984415683</v>
+        <v>11.307280092509769</v>
       </c>
       <c r="E23">
-        <v>43.357949278175646</v>
+        <v>43.474816959427955</v>
       </c>
       <c r="F23">
-        <v>3.7580281671935274</v>
+        <v>3.8448518656778283</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B24">
-        <v>13.738862557574727</v>
+        <v>12.950376125846486</v>
       </c>
       <c r="C24">
-        <v>-18.704924205136475</v>
+        <v>-18.707915158697077</v>
       </c>
       <c r="D24">
-        <v>11.307280092509769</v>
+        <v>11.166528871855119</v>
       </c>
       <c r="E24">
-        <v>43.474816959427955</v>
+        <v>42.194833115750164</v>
       </c>
       <c r="F24">
-        <v>3.8448518656778283</v>
+        <v>3.7786883999468177</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B25">
-        <v>12.950376125846486</v>
+        <v>13.744093948538705</v>
       </c>
       <c r="C25">
-        <v>-18.707915158697077</v>
+        <v>-17.820004267719014</v>
       </c>
       <c r="D25">
-        <v>11.166528871855119</v>
+        <v>11.794637998708891</v>
       </c>
       <c r="E25">
-        <v>42.194833115750164</v>
+        <v>43.29889380266885</v>
       </c>
       <c r="F25">
-        <v>3.7786883999468177</v>
+        <v>3.6710659375394648</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B26">
-        <v>13.744093948538705</v>
+        <v>13.24928095718958</v>
       </c>
       <c r="C26">
-        <v>-17.820004267719014</v>
+        <v>-19.141919476461709</v>
       </c>
       <c r="D26">
-        <v>11.794637998708891</v>
+        <v>10.824096708299805</v>
       </c>
       <c r="E26">
-        <v>43.29889380266885</v>
+        <v>40.93748042527011</v>
       </c>
       <c r="F26">
-        <v>3.6710659375394648</v>
+        <v>3.782068982613549</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B27">
-        <v>13.24928095718958</v>
+        <v>13.284603274104079</v>
       </c>
       <c r="C27">
-        <v>-19.141919476461709</v>
+        <v>-18.82387651853734</v>
       </c>
       <c r="D27">
-        <v>10.824096708299805</v>
+        <v>11.441838330995417</v>
       </c>
       <c r="E27">
-        <v>40.93748042527011</v>
+        <v>42.075213894148185</v>
       </c>
       <c r="F27">
-        <v>3.782068982613549</v>
+        <v>3.6773123930765874</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B28">
-        <v>13.284603274104079</v>
+        <v>11.075983085798935</v>
       </c>
       <c r="C28">
-        <v>-18.82387651853734</v>
+        <v>-17.414532398062121</v>
       </c>
       <c r="D28">
-        <v>11.441838330995417</v>
+        <v>12.419397375975901</v>
       </c>
       <c r="E28">
-        <v>42.075213894148185</v>
+        <v>40.617778175885704</v>
       </c>
       <c r="F28">
-        <v>3.6773123930765874</v>
+        <v>3.2705111968199669</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B29">
-        <v>11.075983085798935</v>
+        <v>11.403820297086753</v>
       </c>
       <c r="C29">
-        <v>-17.414532398062121</v>
+        <v>-16.963180242268283</v>
       </c>
       <c r="D29">
-        <v>12.419397375975901</v>
+        <v>12.753987640839377</v>
       </c>
       <c r="E29">
-        <v>40.617778175885704</v>
+        <v>41.036811026273206</v>
       </c>
       <c r="F29">
-        <v>3.2705111968199669</v>
+        <v>3.2175670999452572</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B30">
-        <v>11.403820297086753</v>
+        <v>9.5944934196710019</v>
       </c>
       <c r="C30">
-        <v>-16.963180242268283</v>
+        <v>-17.244118327083502</v>
       </c>
       <c r="D30">
-        <v>12.753987640839377</v>
+        <v>12.926260045287316</v>
       </c>
       <c r="E30">
-        <v>41.036811026273206</v>
+        <v>41.311532490697516</v>
       </c>
       <c r="F30">
-        <v>3.2175670999452572</v>
+        <v>3.1959385271503153</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B31">
-        <v>9.5944934196710019</v>
+        <v>9.6708309178326068</v>
       </c>
       <c r="C31">
-        <v>-17.244118327083502</v>
+        <v>-18.047732582575414</v>
       </c>
       <c r="D31">
-        <v>12.926260045287316</v>
+        <v>12.984752582468079</v>
       </c>
       <c r="E31">
-        <v>41.311532490697516</v>
+        <v>41.646720732128614</v>
       </c>
       <c r="F31">
-        <v>3.1959385271503153</v>
+        <v>3.2073557403288318</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B32">
-        <v>9.6708309178326068</v>
+        <v>8.8292952676263248</v>
       </c>
       <c r="C32">
-        <v>-18.047732582575414</v>
+        <v>-17.832395353890362</v>
       </c>
       <c r="D32">
-        <v>12.984752582468079</v>
+        <v>13.270863350673102</v>
       </c>
       <c r="E32">
-        <v>41.646720732128614</v>
+        <v>41.604155662060393</v>
       </c>
       <c r="F32">
-        <v>3.2073557403288318</v>
+        <v>3.1349999289948398</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B33">
-        <v>8.8292952676263248</v>
+        <v>10.849679881432372</v>
       </c>
       <c r="C33">
-        <v>-17.832395353890362</v>
+        <v>-17.920592829791858</v>
       </c>
       <c r="D33">
-        <v>13.270863350673102</v>
+        <v>12.956518661410158</v>
       </c>
       <c r="E33">
-        <v>41.604155662060393</v>
+        <v>41.504392544271276</v>
       </c>
       <c r="F33">
-        <v>3.1349999289948398</v>
+        <v>3.203359917034537</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B34">
-        <v>10.849679881432372</v>
+        <v>11.477254185030983</v>
       </c>
       <c r="C34">
-        <v>-17.920592829791858</v>
+        <v>-19.802287220652694</v>
       </c>
       <c r="D34">
-        <v>12.956518661410158</v>
+        <v>11.811693842049992</v>
       </c>
       <c r="E34">
-        <v>41.504392544271276</v>
+        <v>43.839677630982365</v>
       </c>
       <c r="F34">
-        <v>3.203359917034537</v>
+        <v>3.7115487598325454</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B35">
-        <v>11.477254185030983</v>
+        <v>11.458270735504428</v>
       </c>
       <c r="C35">
-        <v>-19.802287220652694</v>
+        <v>-17.889717003831464</v>
       </c>
       <c r="D35">
-        <v>11.811693842049992</v>
+        <v>12.814679191214344</v>
       </c>
       <c r="E35">
-        <v>43.839677630982365</v>
+        <v>42.006314243646365</v>
       </c>
       <c r="F35">
-        <v>3.7115487598325454</v>
+        <v>3.2779840694291908</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B36">
-        <v>11.458270735504428</v>
+        <v>9.0929764298777194</v>
       </c>
       <c r="C36">
-        <v>-17.889717003831464</v>
+        <v>-19.307049677566024</v>
       </c>
       <c r="D36">
-        <v>12.814679191214344</v>
+        <v>12.689047508720904</v>
       </c>
       <c r="E36">
-        <v>42.006314243646365</v>
+        <v>40.92105447726432</v>
       </c>
       <c r="F36">
-        <v>3.2779840694291908</v>
+        <v>3.2249114402905481</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B37">
-        <v>9.0929764298777194</v>
+        <v>11.513408218107646</v>
       </c>
       <c r="C37">
-        <v>-19.307049677566024</v>
+        <v>-18.151078424636815</v>
       </c>
       <c r="D37">
-        <v>12.689047508720904</v>
+        <v>12.360568911308137</v>
       </c>
       <c r="E37">
-        <v>40.92105447726432</v>
+        <v>42.772712007210899</v>
       </c>
       <c r="F37">
-        <v>3.2249114402905481</v>
+        <v>3.4604161276169125</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B38">
-        <v>11.513408218107646</v>
+        <v>9.9048112989743586</v>
       </c>
       <c r="C38">
-        <v>-18.151078424636815</v>
+        <v>-17.084415725017177</v>
       </c>
       <c r="D38">
-        <v>12.360568911308137</v>
+        <v>12.510531296232708</v>
       </c>
       <c r="E38">
-        <v>42.772712007210899</v>
+        <v>41.756268676899232</v>
       </c>
       <c r="F38">
-        <v>3.4604161276169125</v>
+        <v>3.3376894784215345</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B39">
-        <v>9.9048112989743586</v>
+        <v>11.42609796618288</v>
       </c>
       <c r="C39">
-        <v>-17.084415725017177</v>
+        <v>-18.224776417272494</v>
       </c>
       <c r="D39">
-        <v>12.510531296232708</v>
+        <v>12.60274355698161</v>
       </c>
       <c r="E39">
-        <v>41.756268676899232</v>
+        <v>41.689670146663957</v>
       </c>
       <c r="F39">
-        <v>3.3376894784215345</v>
+        <v>3.3079836908661768</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B40">
-        <v>11.42609796618288</v>
+        <v>9.365438580633878</v>
       </c>
       <c r="C40">
-        <v>-18.224776417272494</v>
+        <v>-19.083857347066413</v>
       </c>
       <c r="D40">
-        <v>12.60274355698161</v>
+        <v>12.776828091337824</v>
       </c>
       <c r="E40">
-        <v>41.689670146663957</v>
+        <v>40.464003830933976</v>
       </c>
       <c r="F40">
-        <v>3.3079836908661768</v>
+        <v>3.1669835065220093</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B41">
-        <v>9.365438580633878</v>
+        <v>8.6757983230358882</v>
       </c>
       <c r="C41">
-        <v>-19.083857347066413</v>
+        <v>-19.109542986298855</v>
       </c>
       <c r="D41">
-        <v>12.776828091337824</v>
+        <v>12.929943879124723</v>
       </c>
       <c r="E41">
-        <v>40.464003830933976</v>
+        <v>41.454084526930927</v>
       </c>
       <c r="F41">
-        <v>3.1669835065220093</v>
+        <v>3.2060529352999105</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B42">
-        <v>8.6757983230358882</v>
+        <v>10.329278346337123</v>
       </c>
       <c r="C42">
-        <v>-19.109542986298855</v>
+        <v>-19.63518333667502</v>
       </c>
       <c r="D42">
-        <v>12.929943879124723</v>
+        <v>12.208696527602038</v>
       </c>
       <c r="E42">
-        <v>41.454084526930927</v>
+        <v>39.947805553544875</v>
       </c>
       <c r="F42">
-        <v>3.2060529352999105</v>
+        <v>3.2720778555867005</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B43">
-        <v>10.329278346337123</v>
+        <v>9.5736854774615132</v>
       </c>
       <c r="C43">
-        <v>-19.63518333667502</v>
+        <v>-18.832043318622425</v>
       </c>
       <c r="D43">
-        <v>12.208696527602038</v>
+        <v>11.677124815681291</v>
       </c>
       <c r="E43">
-        <v>39.947805553544875</v>
+        <v>42.718820850399041</v>
       </c>
       <c r="F43">
-        <v>3.2720778555867005</v>
+        <v>3.6583338385688613</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B44">
-        <v>9.5736854774615132</v>
+        <v>11.191571531960598</v>
       </c>
       <c r="C44">
-        <v>-18.832043318622425</v>
+        <v>-17.411081582341168</v>
       </c>
       <c r="D44">
-        <v>11.677124815681291</v>
+        <v>11.882343935858936</v>
       </c>
       <c r="E44">
-        <v>42.718820850399041</v>
+        <v>37.673531338945274</v>
       </c>
       <c r="F44">
-        <v>3.6583338385688613</v>
+        <v>3.170547119516784</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B45">
-        <v>11.191571531960598</v>
+        <v>9.1145853134801946</v>
       </c>
       <c r="C45">
-        <v>-17.411081582341168</v>
+        <v>-18.451213957898283</v>
       </c>
       <c r="D45">
-        <v>11.882343935858936</v>
+        <v>13.582484514888586</v>
       </c>
       <c r="E45">
-        <v>37.673531338945274</v>
+        <v>43.686771445665244</v>
       </c>
       <c r="F45">
-        <v>3.170547119516784</v>
+        <v>3.216405024999478</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B46">
-        <v>9.1145853134801946</v>
+        <v>10.533056371546223</v>
       </c>
       <c r="C46">
-        <v>-18.451213957898283</v>
+        <v>-18.358438988486768</v>
       </c>
       <c r="D46">
-        <v>13.582484514888586</v>
+        <v>12.388334401353193</v>
       </c>
       <c r="E46">
-        <v>43.686771445665244</v>
+        <v>39.865156997464297</v>
       </c>
       <c r="F46">
-        <v>3.216405024999478</v>
+        <v>3.2179593887221656</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B47">
-        <v>10.533056371546223</v>
+        <v>10.922594875232949</v>
       </c>
       <c r="C47">
-        <v>-18.358438988486768</v>
+        <v>-17.775742620103728</v>
       </c>
       <c r="D47">
-        <v>12.388334401353193</v>
+        <v>9.9723364599268276</v>
       </c>
       <c r="E47">
-        <v>39.865156997464297</v>
+        <v>33.669819467061885</v>
       </c>
       <c r="F47">
-        <v>3.2179593887221656</v>
+        <v>3.3763220487357022</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B48">
-        <v>10.922594875232949</v>
+        <v>9.6198825748130545</v>
       </c>
       <c r="C48">
-        <v>-17.775742620103728</v>
+        <v>-18.02767490047863</v>
       </c>
       <c r="D48">
-        <v>9.9723364599268276</v>
+        <v>12.667489452125404</v>
       </c>
       <c r="E48">
-        <v>33.669819467061885</v>
+        <v>41.995105663651323</v>
       </c>
       <c r="F48">
-        <v>3.3763220487357022</v>
+        <v>3.3151877348992156</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B49">
-        <v>9.6198825748130545</v>
+        <v>10.648911709048914</v>
       </c>
       <c r="C49">
-        <v>-18.02767490047863</v>
+        <v>-18.601816759345134</v>
       </c>
       <c r="D49">
-        <v>12.667489452125404</v>
+        <v>11.580346780523096</v>
       </c>
       <c r="E49">
-        <v>41.995105663651323</v>
+        <v>44.214762510572363</v>
       </c>
       <c r="F49">
-        <v>3.3151877348992156</v>
+        <v>3.8180862238889826</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B50">
-        <v>10.648911709048914</v>
+        <v>10.379049330484946</v>
       </c>
       <c r="C50">
-        <v>-18.601816759345134</v>
+        <v>-18.105483996166292</v>
       </c>
       <c r="D50">
-        <v>11.580346780523096</v>
+        <v>11.802017713285764</v>
       </c>
       <c r="E50">
-        <v>44.214762510572363</v>
+        <v>42.988975695048516</v>
       </c>
       <c r="F50">
-        <v>3.8180862238889826</v>
+        <v>3.6425106909181282</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B51">
-        <v>10.379049330484946</v>
+        <v>10.952751182600862</v>
       </c>
       <c r="C51">
-        <v>-18.105483996166292</v>
+        <v>-18.259573508744076</v>
       </c>
       <c r="D51">
-        <v>11.802017713285764</v>
+        <v>11.803803322179096</v>
       </c>
       <c r="E51">
-        <v>42.988975695048516</v>
+        <v>42.297362468122053</v>
       </c>
       <c r="F51">
-        <v>3.6425106909181282</v>
+        <v>3.5833672684672919</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B52">
-        <v>10.952751182600862</v>
+        <v>10.121268185981691</v>
       </c>
       <c r="C52">
-        <v>-18.259573508744076</v>
+        <v>-17.227930355313337</v>
       </c>
       <c r="D52">
-        <v>11.803803322179096</v>
+        <v>12.61810984866012</v>
       </c>
       <c r="E52">
-        <v>42.297362468122053</v>
+        <v>40.541298633111651</v>
       </c>
       <c r="F52">
-        <v>3.5833672684672919</v>
+        <v>3.2129454505752788</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B53">
-        <v>10.121268185981691</v>
+        <v>9.9558165154063349</v>
       </c>
       <c r="C53">
-        <v>-17.227930355313337</v>
+        <v>-17.583405342055379</v>
       </c>
       <c r="D53">
-        <v>12.61810984866012</v>
+        <v>12.382557431388298</v>
       </c>
       <c r="E53">
-        <v>40.541298633111651</v>
+        <v>41.55194500791665</v>
       </c>
       <c r="F53">
-        <v>3.2129454505752788</v>
+        <v>3.3556836088308746</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B54">
-        <v>9.9558165154063349</v>
+        <v>9.8908187565847072</v>
       </c>
       <c r="C54">
-        <v>-17.583405342055379</v>
+        <v>-19.969322781341337</v>
       </c>
       <c r="D54">
-        <v>12.382557431388298</v>
+        <v>12.265789848909858</v>
       </c>
       <c r="E54">
-        <v>41.55194500791665</v>
+        <v>39.713199099131984</v>
       </c>
       <c r="F54">
-        <v>3.3556836088308746</v>
+        <v>3.2377204883109552</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B55">
-        <v>9.8908187565847072</v>
+        <v>9.5963122856179695</v>
       </c>
       <c r="C55">
-        <v>-19.969322781341337</v>
+        <v>-18.174012481124933</v>
       </c>
       <c r="D55">
-        <v>12.265789848909858</v>
+        <v>12.047094201643368</v>
       </c>
       <c r="E55">
-        <v>39.713199099131984</v>
+        <v>41.713898246585671</v>
       </c>
       <c r="F55">
-        <v>3.2377204883109552</v>
+        <v>3.4625692759084923</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B56">
-        <v>9.5963122856179695</v>
+        <v>10.156393880855319</v>
       </c>
       <c r="C56">
-        <v>-18.174012481124933</v>
+        <v>-17.567936071484212</v>
       </c>
       <c r="D56">
-        <v>12.047094201643368</v>
+        <v>12.539616038156367</v>
       </c>
       <c r="E56">
-        <v>41.713898246585671</v>
+        <v>41.620408714712944</v>
       </c>
       <c r="F56">
-        <v>3.4625692759084923</v>
+        <v>3.3191134870531624</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B57">
-        <v>10.156393880855319</v>
+        <v>9.7201557216677337</v>
       </c>
       <c r="C57">
-        <v>-17.567936071484212</v>
+        <v>-18.534592065878599</v>
       </c>
       <c r="D57">
-        <v>12.539616038156367</v>
+        <v>11.155919138815362</v>
       </c>
       <c r="E57">
-        <v>41.620408714712944</v>
+        <v>39.120792323343153</v>
       </c>
       <c r="F57">
-        <v>3.3191134870531624</v>
+        <v>3.506729641597004</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B58">
-        <v>9.7201557216677337</v>
+        <v>11.269978996145458</v>
       </c>
       <c r="C58">
-        <v>-18.534592065878599</v>
+        <v>-17.800002800980597</v>
       </c>
       <c r="D58">
-        <v>11.155919138815362</v>
+        <v>12.868373053272588</v>
       </c>
       <c r="E58">
-        <v>39.120792323343153</v>
+        <v>40.579143014722682</v>
       </c>
       <c r="F58">
-        <v>3.506729641597004</v>
+        <v>3.1534011989497692</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B59">
-        <v>11.269978996145458</v>
+        <v>11.038218576943981</v>
       </c>
       <c r="C59">
-        <v>-17.800002800980597</v>
+        <v>-17.591436199861032</v>
       </c>
       <c r="D59">
-        <v>12.868373053272588</v>
+        <v>12.493666309166194</v>
       </c>
       <c r="E59">
-        <v>40.579143014722682</v>
+        <v>39.938482513142276</v>
       </c>
       <c r="F59">
-        <v>3.1534011989497692</v>
+        <v>3.196698352975917</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B60">
-        <v>11.038218576943981</v>
+        <v>10.959011668531415</v>
       </c>
       <c r="C60">
-        <v>-17.591436199861032</v>
+        <v>-19.203629269082256</v>
       </c>
       <c r="D60">
-        <v>12.493666309166194</v>
+        <v>11.1300640982691</v>
       </c>
       <c r="E60">
-        <v>39.938482513142276</v>
+        <v>38.52263717977322</v>
       </c>
       <c r="F60">
-        <v>3.196698352975917</v>
+        <v>3.4611334525705106</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B61">
-        <v>10.959011668531415</v>
+        <v>11.222304673515815</v>
       </c>
       <c r="C61">
-        <v>-19.203629269082256</v>
+        <v>-16.950396401669508</v>
       </c>
       <c r="D61">
-        <v>11.1300640982691</v>
+        <v>12.252697720061217</v>
       </c>
       <c r="E61">
-        <v>38.52263717977322</v>
+        <v>41.305861865011224</v>
       </c>
       <c r="F61">
-        <v>3.4611334525705106</v>
+        <v>3.3711646862373463</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B62">
-        <v>11.222304673515815</v>
+        <v>10.506473134191285</v>
       </c>
       <c r="C62">
-        <v>-16.950396401669508</v>
+        <v>-18.590031396161557</v>
       </c>
       <c r="D62">
-        <v>12.252697720061217</v>
+        <v>11.577622420495404</v>
       </c>
       <c r="E62">
-        <v>41.305861865011224</v>
+        <v>37.632625486158439</v>
       </c>
       <c r="F62">
-        <v>3.3711646862373463</v>
+        <v>3.2504623245908331</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B63">
-        <v>10.506473134191285</v>
+        <v>11.373110989707946</v>
       </c>
       <c r="C63">
-        <v>-18.590031396161557</v>
+        <v>-17.664434365490365</v>
       </c>
       <c r="D63">
-        <v>11.577622420495404</v>
+        <v>12.776327105198735</v>
       </c>
       <c r="E63">
-        <v>37.632625486158439</v>
+        <v>41.681607581177502</v>
       </c>
       <c r="F63">
-        <v>3.2504623245908331</v>
+        <v>3.2624092384279284</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B64">
-        <v>11.373110989707946</v>
+        <v>10.313614451342712</v>
       </c>
       <c r="C64">
-        <v>-17.664434365490365</v>
+        <v>-17.554957193306908</v>
       </c>
       <c r="D64">
-        <v>12.776327105198735</v>
+        <v>11.410585080733936</v>
       </c>
       <c r="E64">
-        <v>41.681607581177502</v>
+        <v>43.147884939664692</v>
       </c>
       <c r="F64">
-        <v>3.2624092384279284</v>
+        <v>3.7813911060982504</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B65">
-        <v>10.313614451342712</v>
+        <v>9.8549182157241511</v>
       </c>
       <c r="C65">
-        <v>-17.554957193306908</v>
+        <v>-18.519739096946264</v>
       </c>
       <c r="D65">
-        <v>11.410585080733936</v>
+        <v>8.6335783175948038</v>
       </c>
       <c r="E65">
-        <v>43.147884939664692</v>
+        <v>27.98987812019848</v>
       </c>
       <c r="F65">
-        <v>3.7813911060982504</v>
+        <v>3.2419788285416371</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B66">
-        <v>9.8549182157241511</v>
+        <v>11.268502424374827</v>
       </c>
       <c r="C66">
-        <v>-18.519739096946264</v>
+        <v>-17.594274480314141</v>
       </c>
       <c r="D66">
-        <v>8.6335783175948038</v>
+        <v>12.291026070945932</v>
       </c>
       <c r="E66">
-        <v>27.98987812019848</v>
+        <v>39.083508754891348</v>
       </c>
       <c r="F66">
-        <v>3.2419788285416371</v>
+        <v>3.1798410099608092</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B67">
-        <v>11.268502424374827</v>
+        <v>10.23058205316385</v>
       </c>
       <c r="C67">
-        <v>-17.594274480314141</v>
+        <v>-17.16046232015578</v>
       </c>
       <c r="D67">
-        <v>12.291026070945932</v>
+        <v>12.619984253223331</v>
       </c>
       <c r="E67">
-        <v>39.083508754891348</v>
+        <v>40.542385725778814</v>
       </c>
       <c r="F67">
-        <v>3.1798410099608092</v>
+        <v>3.2125543829758496</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B68">
-        <v>10.23058205316385</v>
+        <v>12.378219238452504</v>
       </c>
       <c r="C68">
-        <v>-17.16046232015578</v>
+        <v>-16.833149676385606</v>
       </c>
       <c r="D68">
-        <v>12.619984253223331</v>
+        <v>13.0535780634214</v>
       </c>
       <c r="E68">
-        <v>40.542385725778814</v>
+        <v>40.685420910858433</v>
       </c>
       <c r="F68">
-        <v>3.2125543829758496</v>
+        <v>3.1168022065051035</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B69">
-        <v>12.378219238452504</v>
+        <v>9.6227821941081704</v>
       </c>
       <c r="C69">
-        <v>-16.833149676385606</v>
+        <v>-17.476381764716777</v>
       </c>
       <c r="D69">
-        <v>13.0535780634214</v>
+        <v>11.391888111174337</v>
       </c>
       <c r="E69">
-        <v>40.685420910858433</v>
+        <v>40.567746703909073</v>
       </c>
       <c r="F69">
-        <v>3.1168022065051035</v>
+        <v>3.561108247202327</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B70">
-        <v>9.6227821941081704</v>
+        <v>11.022622725389564</v>
       </c>
       <c r="C70">
-        <v>-17.476381764716777</v>
+        <v>-16.949020950909556</v>
       </c>
       <c r="D70">
-        <v>11.391888111174337</v>
+        <v>12.798601088502553</v>
       </c>
       <c r="E70">
-        <v>40.567746703909073</v>
+        <v>40.156738239825778</v>
       </c>
       <c r="F70">
-        <v>3.561108247202327</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>77</v>
-      </c>
-      <c r="B71">
-        <v>11.022622725389564</v>
-      </c>
-      <c r="C71">
-        <v>-16.949020950909556</v>
-      </c>
-      <c r="D71">
-        <v>12.798601088502553</v>
-      </c>
-      <c r="E71">
-        <v>40.156738239825778</v>
-      </c>
-      <c r="F71">
         <v>3.137588081864668</v>
       </c>
     </row>

</xml_diff>